<commit_message>
readme + error analysis results
</commit_message>
<xml_diff>
--- a/ErrorAnalysisResults.xlsx
+++ b/ErrorAnalysisResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiam\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\NLP Project\Repository\squad-nlp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16187BA-F563-473A-9D66-8B9E1B54C9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E6BA23-44C7-444C-A861-945ABE3961B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
   <si>
     <t>Question</t>
   </si>
@@ -29,21 +29,6 @@
   </si>
   <si>
     <t>Exact Answer</t>
-  </si>
-  <si>
-    <t>Glove Baseline Answer</t>
-  </si>
-  <si>
-    <t>Glove + Features Answer</t>
-  </si>
-  <si>
-    <t>Glove + Attention Answer</t>
-  </si>
-  <si>
-    <t>Glove + Char + Attention Answer</t>
-  </si>
-  <si>
-    <t>Bert Answer</t>
   </si>
   <si>
     <t>What did Irvin Rock write about?</t>
@@ -186,9 +171,6 @@
     <t>educational establishments,</t>
   </si>
   <si>
-    <t>Modello</t>
-  </si>
-  <si>
     <t>Error Ans (%)</t>
   </si>
   <si>
@@ -211,13 +193,34 @@
   </si>
   <si>
     <t>Bert</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>GloVe Baseline Answer</t>
+  </si>
+  <si>
+    <t>GloVe + Features Answer</t>
+  </si>
+  <si>
+    <t>GloVe + Attention Answer</t>
+  </si>
+  <si>
+    <t>GloVe + Char + Attention Answer</t>
+  </si>
+  <si>
+    <t>BERT Answer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -241,6 +244,50 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -362,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -374,9 +421,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -396,15 +440,46 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -626,124 +701,130 @@
   </sheetPr>
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38.85546875" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
-    <col min="8" max="9" width="24.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.6640625" style="25" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" customWidth="1"/>
+    <col min="9" max="9" width="26.6640625" customWidth="1"/>
+    <col min="10" max="10" width="22.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:10" s="30" customFormat="1" ht="46.2" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="29"/>
+      <c r="E1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="228" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F1" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="228" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="16" t="s">
+        <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="242.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="242.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="I3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="117.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="117.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="3">
+        <v>15</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="17">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G4" s="3">
         <v>6.3E-2</v>
@@ -758,112 +839,112 @@
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="104.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="104.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="I5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="14"/>
-      <c r="E5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>29</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="105.6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="16" t="s">
+        <v>26</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="I6" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="I7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="J7" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="218.1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="218.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="2">
+        <v>37</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="16">
         <v>1680</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G8" s="2">
         <v>1680</v>
@@ -878,216 +959,216 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="218.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="218.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="I9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="19"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B11" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="18"/>
-      <c r="E9" s="5" t="s">
+      <c r="D11" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="E11" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="C12" s="9">
+        <v>92.9</v>
+      </c>
+      <c r="D12" s="9">
+        <v>2.27</v>
+      </c>
+      <c r="E12" s="21">
+        <v>4.83</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B11" s="8" t="s">
+      <c r="C13" s="10">
+        <v>60.64</v>
+      </c>
+      <c r="D13" s="10">
+        <v>12.63</v>
+      </c>
+      <c r="E13" s="22">
+        <v>26.73</v>
+      </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C14" s="10">
+        <v>43.23</v>
+      </c>
+      <c r="D14" s="9">
+        <v>16.41</v>
+      </c>
+      <c r="E14" s="21">
+        <v>40.36</v>
+      </c>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="C15" s="9">
+        <v>42.38</v>
+      </c>
+      <c r="D15" s="9">
+        <v>15.89</v>
+      </c>
+      <c r="E15" s="21">
+        <v>41.74</v>
+      </c>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B12" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="10">
-        <v>92.9</v>
-      </c>
-      <c r="D12" s="10">
-        <v>2.27</v>
-      </c>
-      <c r="E12" s="10">
-        <v>4.83</v>
-      </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-    </row>
-    <row r="13" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="11">
-        <v>60.64</v>
-      </c>
-      <c r="D13" s="11">
-        <v>12.63</v>
-      </c>
-      <c r="E13" s="11">
-        <v>26.73</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B14" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="11">
-        <v>43.23</v>
-      </c>
-      <c r="D14" s="10">
-        <v>16.41</v>
-      </c>
-      <c r="E14" s="10">
-        <v>40.36</v>
-      </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-    </row>
-    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="10">
-        <v>42.38</v>
-      </c>
-      <c r="D15" s="10">
-        <v>15.89</v>
-      </c>
-      <c r="E15" s="10">
-        <v>41.74</v>
-      </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B16" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C16" s="10">
+      <c r="C16" s="9">
         <v>30.01</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="9">
         <v>12.85</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="21">
         <v>57.13</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-    </row>
-    <row r="18" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-    </row>
-    <row r="19" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-    </row>
-    <row r="20" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-    </row>
-    <row r="21" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-    </row>
-    <row r="22" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-    </row>
-    <row r="23" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1102,5 +1183,6 @@
     <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>